<commit_message>
adicionando usuario ao banco
</commit_message>
<xml_diff>
--- a/Sprint 1.xlsx
+++ b/Sprint 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pucpredu-my.sharepoint.com/personal/lucas_fritsche1_grupomarista_org_br/Documents/Desktop/Aulas/Exp Criativa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{2D434FFA-569C-4E53-94EA-F317BA4DEB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7928CA83-7470-45D4-81BF-B3CAFAA094E7}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{2D434FFA-569C-4E53-94EA-F317BA4DEB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABA34C8C-EFEE-4731-8CFE-20B07922720E}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7270" xr2:uid="{FF344253-DE22-4546-9D67-076E6E10C3AC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FF344253-DE22-4546-9D67-076E6E10C3AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -493,7 +493,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -547,7 +547,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>

</xml_diff>